<commit_message>
All testcases are working
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetBanking/testData/LoginData.xlsx
+++ b/src/test/java/com/inetBanking/testData/LoginData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="18732" windowHeight="7992"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="18396" windowHeight="9252"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,16 +32,16 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr296371</t>
-  </si>
-  <si>
-    <t>zezynaj</t>
-  </si>
-  <si>
     <t>sepygUb</t>
   </si>
   <si>
     <t>mngr303136</t>
+  </si>
+  <si>
+    <t>mngr302125</t>
+  </si>
+  <si>
+    <t>pAjapEq</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,18 +387,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>